<commit_message>
update plan 20201118 & update result 20201117
</commit_message>
<xml_diff>
--- a/20201117.xlsx
+++ b/20201117.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swan3\Desktop\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A0B50A7-A70C-4A90-8434-7086C3E11FA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D595B5-097B-491D-8166-2482CEA77A76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-120" windowWidth="23256" windowHeight="12576" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23844" yWindow="1152" windowWidth="21600" windowHeight="11328" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="59">
   <si>
     <t>일</t>
   </si>
@@ -197,10 +197,6 @@
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
   <si>
-    <t>일일업무</t>
-    <phoneticPr fontId="21" type="noConversion"/>
-  </si>
-  <si>
     <t>회원정보 조회실패, 비상정지 UI수정</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
@@ -214,6 +210,42 @@
   </si>
   <si>
     <t>1시30분 취침 지키기</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>F7
+ - UI 수정
+  -&gt; EMG화면 적용 (이미지 배경이 투명색으로 적용이 안되어있음, 흰색)
+  -&gt; 회원정보조회 텍스트 적용
+   =&gt; 기존 에러화면+에러코드에서 "회원정보 실패"문구 출력으로 변경
+Mobilty 
+ - MAX13485 3.3v -&gt; 5v로 수정 (2ea피앤이에 전달 후 수정 안 된 버전 2ea 수령 예정)
+  -&gt; 1set만 교환하였음
+ - 피앤이에서 테스트 도중 overrun에러가 빈번하게 발생하여, uart3의 overrun에러를 무시하도록
+   변경하였음
+2채널
+ - 펌웨어 다운로드(1ea, 불량1ea에 대해 MLT에서 교환 받은 제품)
+  -&gt; 2ea추가 불량 교체 예정</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>늦게자고 늦게일어남</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>늦게일어남</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>못했음</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>요즘은 회사에서 작성함</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
 </sst>
@@ -387,7 +419,7 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -601,6 +633,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -907,7 +951,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -953,7 +997,16 @@
     <xf numFmtId="0" fontId="0" fillId="32" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="34" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -965,6 +1018,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="1" fillId="32" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -974,25 +1033,22 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="32" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="32" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1528,7 +1584,7 @@
   <dimension ref="B2:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="F3" sqref="F3:F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1558,7 +1614,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>35</v>
@@ -1581,17 +1637,21 @@
       </c>
     </row>
     <row r="3" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="16" t="s">
-        <v>53</v>
+      <c r="D3" s="28"/>
+      <c r="E3" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>52</v>
       </c>
       <c r="H3" s="11"/>
       <c r="I3" t="s">
@@ -1605,12 +1665,12 @@
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="23"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="27"/>
       <c r="F4" s="23"/>
-      <c r="G4" s="17"/>
+      <c r="G4" s="20"/>
       <c r="H4" s="11"/>
       <c r="I4" t="s">
         <v>18</v>
@@ -1620,12 +1680,12 @@
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="23"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="27"/>
       <c r="F5" s="23"/>
-      <c r="G5" s="17"/>
+      <c r="G5" s="20"/>
       <c r="H5" s="11"/>
       <c r="I5" t="s">
         <v>19</v>
@@ -1635,12 +1695,12 @@
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="23"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="27"/>
       <c r="F6" s="23"/>
-      <c r="G6" s="17"/>
+      <c r="G6" s="20"/>
       <c r="H6" s="11"/>
       <c r="I6" t="s">
         <v>17</v>
@@ -1650,12 +1710,12 @@
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="23"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="27"/>
       <c r="F7" s="23"/>
-      <c r="G7" s="17"/>
+      <c r="G7" s="20"/>
       <c r="H7" s="11"/>
       <c r="I7" t="s">
         <v>14</v>
@@ -1669,12 +1729,12 @@
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="23"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="27"/>
       <c r="F8" s="23"/>
-      <c r="G8" s="17"/>
+      <c r="G8" s="20"/>
       <c r="H8" s="11"/>
       <c r="I8" t="s">
         <v>6</v>
@@ -1690,10 +1750,12 @@
       <c r="C9" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="5"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="17" t="s">
+        <v>56</v>
+      </c>
       <c r="F9" s="23"/>
-      <c r="G9" s="17"/>
+      <c r="G9" s="20"/>
       <c r="H9" s="11"/>
       <c r="I9" t="s">
         <v>8</v>
@@ -1712,23 +1774,23 @@
       <c r="C10" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="15"/>
+      <c r="D10" s="31"/>
       <c r="E10" s="14"/>
       <c r="F10" s="23"/>
-      <c r="G10" s="17"/>
+      <c r="G10" s="20"/>
       <c r="H10" s="11"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="15"/>
+      <c r="C11" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="31"/>
       <c r="E11" s="5"/>
       <c r="F11" s="23"/>
-      <c r="G11" s="17"/>
+      <c r="G11" s="20"/>
       <c r="H11" s="11"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
@@ -1738,10 +1800,10 @@
       <c r="C12" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="15"/>
+      <c r="D12" s="31"/>
       <c r="E12" s="14"/>
       <c r="F12" s="23"/>
-      <c r="G12" s="17"/>
+      <c r="G12" s="20"/>
       <c r="H12" s="11"/>
     </row>
     <row r="13" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1749,12 +1811,12 @@
         <v>26</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="15"/>
+        <v>50</v>
+      </c>
+      <c r="D13" s="31"/>
       <c r="E13" s="5"/>
       <c r="F13" s="23"/>
-      <c r="G13" s="17"/>
+      <c r="G13" s="20"/>
       <c r="H13" s="11"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
@@ -1764,10 +1826,10 @@
       <c r="C14" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="15"/>
+      <c r="D14" s="31"/>
       <c r="E14" s="14"/>
       <c r="F14" s="23"/>
-      <c r="G14" s="17"/>
+      <c r="G14" s="20"/>
       <c r="H14" s="11"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
@@ -1775,12 +1837,12 @@
         <v>29</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="15"/>
+        <v>50</v>
+      </c>
+      <c r="D15" s="31"/>
       <c r="E15" s="5"/>
       <c r="F15" s="23"/>
-      <c r="G15" s="17"/>
+      <c r="G15" s="20"/>
       <c r="H15" s="11"/>
     </row>
     <row r="16" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1790,10 +1852,10 @@
       <c r="C16" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="15"/>
+      <c r="D16" s="31"/>
       <c r="E16" s="14"/>
       <c r="F16" s="23"/>
-      <c r="G16" s="17"/>
+      <c r="G16" s="20"/>
       <c r="H16" s="11"/>
     </row>
     <row r="17" spans="2:8" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1801,12 +1863,12 @@
         <v>33</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="15"/>
+        <v>50</v>
+      </c>
+      <c r="D17" s="31"/>
       <c r="E17" s="5"/>
       <c r="F17" s="23"/>
-      <c r="G17" s="17"/>
+      <c r="G17" s="20"/>
       <c r="H17" s="11"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
@@ -1814,12 +1876,12 @@
         <v>41</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="15"/>
+        <v>51</v>
+      </c>
+      <c r="D18" s="31"/>
       <c r="E18" s="14"/>
       <c r="F18" s="23"/>
-      <c r="G18" s="17"/>
+      <c r="G18" s="20"/>
       <c r="H18" s="11"/>
     </row>
     <row r="19" spans="2:8" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1829,10 +1891,10 @@
       <c r="C19" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="15"/>
+      <c r="D19" s="31"/>
       <c r="E19" s="5"/>
       <c r="F19" s="23"/>
-      <c r="G19" s="17"/>
+      <c r="G19" s="20"/>
       <c r="H19" s="11"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
@@ -1842,23 +1904,25 @@
       <c r="C20" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="15"/>
-      <c r="E20" s="14"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="32" t="s">
+        <v>57</v>
+      </c>
       <c r="F20" s="23"/>
-      <c r="G20" s="17"/>
+      <c r="G20" s="20"/>
       <c r="H20" s="11"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="15"/>
+      <c r="D21" s="31"/>
       <c r="E21" s="5"/>
       <c r="F21" s="23"/>
-      <c r="G21" s="17"/>
+      <c r="G21" s="20"/>
       <c r="H21" s="11"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
@@ -1868,10 +1932,10 @@
       <c r="C22" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="15"/>
+      <c r="D22" s="31"/>
       <c r="E22" s="14"/>
       <c r="F22" s="23"/>
-      <c r="G22" s="17"/>
+      <c r="G22" s="20"/>
       <c r="H22" s="11"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
@@ -1881,10 +1945,10 @@
       <c r="C23" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="15"/>
-      <c r="E23" s="27"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="17"/>
       <c r="F23" s="23"/>
-      <c r="G23" s="17"/>
+      <c r="G23" s="20"/>
       <c r="H23" s="11"/>
     </row>
     <row r="24" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1894,13 +1958,18 @@
       <c r="C24" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="15"/>
-      <c r="E24" s="28"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="18" t="s">
+        <v>58</v>
+      </c>
       <c r="F24" s="23"/>
-      <c r="G24" s="18"/>
+      <c r="G24" s="21"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
+      <c r="F25" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>